<commit_message>
Big updates to distractmaps
</commit_message>
<xml_diff>
--- a/fMRI Tasks/WASABI distractmap/N-back-2.xlsx
+++ b/fMRI Tasks/WASABI distractmap/N-back-2.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox (Dartmouth College)\CANLab Projects\WASABI\Paradigms\WASABI_Expectancy_and_Distraction\WASABI Distraction Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\WASABI distractmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34274D93-923C-4E14-9D42-9CEE8923F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B814E9A9-4568-4AA0-A219-8D1DD52C6FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="24285" windowWidth="28110" windowHeight="16065" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="285" windowWidth="38640" windowHeight="22650" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Part1 1-back" sheetId="3" r:id="rId3"/>
-    <sheet name="Part2 2-back" sheetId="5" r:id="rId4"/>
+    <sheet name="Square Locations" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Part1 1-back" sheetId="3" r:id="rId4"/>
     <sheet name="Part3 1-back" sheetId="4" r:id="rId5"/>
+    <sheet name="Part2 2-back" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet7" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet8" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet9" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet10" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet11" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="13">
   <si>
     <t>location</t>
   </si>
@@ -434,11 +443,651 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A654245D-565F-4F2D-A69B-F8D17852FB25}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB12697-CEC1-41A4-873F-9BDD5F5B0539}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, -0.2]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41DA72A-1C6A-468C-BC13-92D3C9D023CE}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D667510-CB3F-4A1E-BA66-23EE0B682780}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6D3709-AC25-4EAE-869E-97860E79D5E5}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE733714-A939-465B-8ABA-7DF54E2AFF95}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +2143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -1860,7 +2509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1F8A58-EA73-4E8C-89E5-6717F4C0D351}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2122,12 +2771,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8609755-E30B-417D-80EF-3FA7A8BD1CDD}">
-  <dimension ref="A1:C57"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB817C21-16FE-4057-8754-28F8C8E9CACE}">
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,44 +2794,48 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f>IF(A3=A2, 1, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <f>IF(A4=A2, 1, 0)</f>
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A3, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C57" si="0">IF(A5=A3, 1, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -2191,7 +2844,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -2200,56 +2853,60 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f>IF(A10=A9, 1, 0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C11:C15" si="1">IF(A11=A10, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2260,79 +2917,87 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <f>IF(A17=A16, 1, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="C18:C22" si="2">IF(A18=A17, 1, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
+      <c r="C24">
+        <f>IF(A24=A23, 1, 0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C25:C29" si="3">IF(A25=A24, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2341,246 +3006,26 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>6</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>6</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>4</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>8</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>5</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>5</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>8</v>
-      </c>
-      <c r="C56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>5</v>
-      </c>
-      <c r="C57">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2588,12 +3033,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB817C21-16FE-4057-8754-28F8C8E9CACE}">
-  <dimension ref="A1:C29"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8609755-E30B-417D-80EF-3FA7A8BD1CDD}">
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,48 +3056,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <f>IF(A3=A2, 1, 0)</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="0">IF(A4=A3, 1, 0)</f>
+        <f>IF(A4=A2, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C57" si="0">IF(A5=A3, 1, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -2661,7 +3126,11 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -2670,60 +3139,84 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <f>IF(A10=A9, 1, 0)</f>
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C15" si="1">IF(A11=A10, 1, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2731,90 +3224,126 @@
       <c r="A16">
         <v>3</v>
       </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <f>IF(A17=A16, 1, 0)</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, -0.2]</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C22" si="2">IF(A18=A17, 1, 0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="C24">
-        <f>IF(A24=A23, 1, 0)</f>
-        <v>1</v>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C29" si="3">IF(A25=A24, 1, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
       </c>
       <c r="C26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2822,26 +3351,697 @@
       <c r="A27">
         <v>6</v>
       </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
       <c r="C27">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
       </c>
       <c r="C28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, -0.2]</v>
       </c>
       <c r="C29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" t="str">
+        <f>VLOOKUP(A37,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="str">
+        <f>VLOOKUP(A38,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="str">
+        <f>VLOOKUP(A39,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" t="str">
+        <f>VLOOKUP(A40,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="str">
+        <f>VLOOKUP(A41,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="str">
+        <f>VLOOKUP(A42,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="str">
+        <f>VLOOKUP(A43,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="str">
+        <f>VLOOKUP(A44,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="str">
+        <f>VLOOKUP(A45,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46" t="str">
+        <f>VLOOKUP(A46,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0]</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="str">
+        <f>VLOOKUP(A47,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="str">
+        <f>VLOOKUP(A48,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="str">
+        <f>VLOOKUP(A49,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="str">
+        <f>VLOOKUP(A50,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="str">
+        <f>VLOOKUP(A51,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="str">
+        <f>VLOOKUP(A52,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53" t="str">
+        <f>VLOOKUP(A53,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="str">
+        <f>VLOOKUP(A54,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55" t="str">
+        <f>VLOOKUP(A55,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" t="str">
+        <f>VLOOKUP(A56,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" t="str">
+        <f>VLOOKUP(A57,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27CD069-9602-4D4A-A285-FFAC0C11B6A9}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+      <c r="C4">
+        <f>IF(A4=A2, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C8" si="0">IF(A5=A3, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0.2]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C5B82B-6761-4853-9845-81C32F519660}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, 0.2]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92255DE6-AC5A-4362-BE2B-5FEAAA0DE735}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, -0.2]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0.2, 0.2]</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="0">IF(A4=A2, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, -0.2]</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[0, -0.2]</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'Square Locations'!A$1:B$10,2,FALSE)</f>
+        <v>[-0.2, 0]</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>